<commit_message>
Removed IND values for PRIndex
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/LA-PRI/LA-PRI.xlsx
+++ b/Simple_XLS_Importer/data/LA-PRI/LA-PRI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\vm\debian8.2-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\landbook-importers\Simple_XLS_Importer\data\LA-PRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="87">
   <si>
     <t>indicator</t>
   </si>
@@ -76,9 +76,6 @@
     <t>GRC</t>
   </si>
   <si>
-    <t>IND</t>
-  </si>
-  <si>
     <t>IDN</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>Total number of respondants in the country sample is 870 (=100%)</t>
   </si>
   <si>
-    <t>Total number of respondants in the country sample is 2590 (=100%)</t>
-  </si>
-  <si>
     <t>Total number of respondants in the country sample is 883 (=100%)</t>
   </si>
   <si>
@@ -130,9 +124,6 @@
     <t>Total number of respondants in the country sample -- home owners only -- is 647 (=100%)</t>
   </si>
   <si>
-    <t>Total number of respondants in the country sample -- home owners only -- is 2282 (=100%)</t>
-  </si>
-  <si>
     <t>Total number of respondants in the country sample -- home owners only -- is 770 (=100%)</t>
   </si>
   <si>
@@ -157,9 +148,6 @@
     <t>Total number of respondants in the country sample -- home owners only -- is 223 (=100%)</t>
   </si>
   <si>
-    <t>Total number of respondants in the country sample -- home owners only -- is 308 (=100%)</t>
-  </si>
-  <si>
     <t>Total number of respondants in the country sample -- home owners only -- is 113 (=100%)</t>
   </si>
   <si>
@@ -187,9 +175,6 @@
     <t>Total number of respondants in the country sample -- home owners only -- is 148 (=100%, weighted base)</t>
   </si>
   <si>
-    <t>Total number of respondants in the country sample -- home owners only -- is 1008 (=100%, weighted base)</t>
-  </si>
-  <si>
     <t>Total number of respondants in the country sample -- home owners only -- is 377 (=100%, weighted base)</t>
   </si>
   <si>
@@ -214,9 +199,6 @@
     <t>Total number of respondants in the country sample -- Rural home owners only -- is 377 (=100%, weighted base)</t>
   </si>
   <si>
-    <t>Total number of respondants in the country sample -- Rural home owners only -- is 708 (=100%, weighted base)</t>
-  </si>
-  <si>
     <t>Total number of respondants in the country sample -- Rural home owners only -- is 122 (=100%, weighted base)</t>
   </si>
   <si>
@@ -239,9 +221,6 @@
   </si>
   <si>
     <t>Total number of respondants in the country sample -- Urban home owners only -- is 255 (=100%, weighted base)</t>
-  </si>
-  <si>
-    <t>Total number of respondants in the country sample -- Urban home owners only -- is 300 (=100%, weighted base)</t>
   </si>
   <si>
     <t>Total number of respondants in the country sample -- Urban home owners only -- is 119 (=100%, weighted base)</t>
@@ -697,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F163"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="A159" activeCellId="17" sqref="A6:XFD6 A15:XFD15 A24:XFD24 A33:XFD33 A42:XFD42 A51:XFD51 A60:XFD60 A69:XFD69 A78:XFD78 A87:XFD87 A96:XFD96 A105:XFD105 A114:XFD114 A123:XFD123 A132:XFD132 A141:XFD141 A150:XFD150 A159:XFD159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -730,7 +709,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -742,16 +721,16 @@
         <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="9">
-        <f>SUM(D2,D11,D20)</f>
+        <f>SUM(D2,D10,D18)</f>
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -763,16 +742,16 @@
         <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="9">
-        <f t="shared" ref="F3:F10" si="0">SUM(D3,D12,D21)</f>
+        <f>SUM(D3,D11,D19)</f>
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -784,16 +763,16 @@
         <v>82.2</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="9">
-        <f t="shared" si="0"/>
+        <f>SUM(D4,D12,D20)</f>
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -805,16 +784,16 @@
         <v>80.599999999999994</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="9">
-        <f t="shared" si="0"/>
+        <f>SUM(D5,D13,D21)</f>
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -823,19 +802,19 @@
         <v>2017</v>
       </c>
       <c r="D6" s="9">
-        <v>90</v>
+        <v>74.3</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="9">
-        <f t="shared" si="0"/>
+        <f>SUM(D6,D14,D22)</f>
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -844,19 +823,19 @@
         <v>2017</v>
       </c>
       <c r="D7" s="9">
-        <v>74.3</v>
+        <v>67.5</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="9">
-        <f t="shared" si="0"/>
+        <f>SUM(D7,D15,D23)</f>
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -865,19 +844,19 @@
         <v>2017</v>
       </c>
       <c r="D8" s="9">
-        <v>67.5</v>
+        <v>74.7</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="9">
-        <f t="shared" si="0"/>
+        <f>SUM(D8,D16,D24)</f>
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -886,49 +865,45 @@
         <v>2017</v>
       </c>
       <c r="D9" s="9">
-        <v>74.7</v>
+        <v>70.5</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="9">
-        <f t="shared" si="0"/>
+        <f>SUM(D9,D17,D25)</f>
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>2017</v>
+      </c>
+      <c r="D10" s="9">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
         <v>19</v>
-      </c>
-      <c r="C10">
-        <v>2017</v>
-      </c>
-      <c r="D10" s="9">
-        <v>70.5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="9">
-        <f t="shared" si="0"/>
-        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>2017</v>
       </c>
       <c r="D11" s="9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
@@ -936,16 +911,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>2017</v>
       </c>
       <c r="D12" s="9">
-        <v>5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -953,16 +928,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>2017</v>
       </c>
       <c r="D13" s="9">
-        <v>2.2000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
@@ -970,16 +945,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>2017</v>
       </c>
       <c r="D14" s="9">
-        <v>4.4000000000000004</v>
+        <v>7.7</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
@@ -987,16 +962,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>2017</v>
       </c>
       <c r="D15" s="9">
-        <v>4.5999999999999996</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E15" t="s">
         <v>24</v>
@@ -1004,16 +979,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>2017</v>
       </c>
       <c r="D16" s="9">
-        <v>7.7</v>
+        <v>6.4</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
@@ -1021,16 +996,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>2017</v>
       </c>
       <c r="D17" s="9">
-        <v>9.3000000000000007</v>
+        <v>7.5</v>
       </c>
       <c r="E17" t="s">
         <v>26</v>
@@ -1038,1031 +1013,1023 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C18">
         <v>2017</v>
       </c>
       <c r="D18" s="9">
-        <v>6.4</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C19">
         <v>2017</v>
       </c>
       <c r="D19" s="9">
-        <v>7.5</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <v>2017</v>
       </c>
       <c r="D20" s="9">
-        <v>9</v>
+        <v>15.6</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C21">
         <v>2017</v>
       </c>
       <c r="D21" s="9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C22">
         <v>2017</v>
       </c>
       <c r="D22" s="9">
-        <v>15.6</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C23">
         <v>2017</v>
       </c>
       <c r="D23" s="9">
-        <v>15</v>
+        <v>23.2</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C24">
         <v>2017</v>
       </c>
       <c r="D24" s="9">
-        <v>5.4</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C25">
         <v>2017</v>
       </c>
       <c r="D25" s="9">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C26">
         <v>2017</v>
       </c>
       <c r="D26" s="9">
-        <v>23.2</v>
+        <v>86.9</v>
       </c>
       <c r="E26" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="F26" s="9">
+        <f>SUM(D26,D34,D42)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C27">
         <v>2017</v>
       </c>
       <c r="D27" s="9">
-        <v>18.899999999999999</v>
+        <v>85.3</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="F27" s="9">
+        <f>SUM(D27,D35,D43)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C28">
         <v>2017</v>
       </c>
       <c r="D28" s="9">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="F28" s="9">
+        <f>SUM(D28,D36,D44)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>2017</v>
       </c>
       <c r="D29" s="9">
-        <v>86.9</v>
+        <v>89</v>
       </c>
       <c r="E29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F29" s="9">
-        <f>SUM(D29,D38,D47)</f>
+        <f>SUM(D29,D37,D45)</f>
         <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C30">
         <v>2017</v>
       </c>
-      <c r="D30" s="9">
-        <v>85.3</v>
+      <c r="D30" s="10">
+        <v>81.599999999999994</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F30" s="9">
-        <f t="shared" ref="F30:F37" si="1">SUM(D30,D39,D48)</f>
+        <f>SUM(D30,D38,D46)</f>
         <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C31">
         <v>2017</v>
       </c>
       <c r="D31" s="9">
-        <v>92</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="E31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F31" s="9">
-        <f t="shared" si="1"/>
+        <f>SUM(D31,D39,D47)</f>
         <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C32">
         <v>2017</v>
       </c>
       <c r="D32" s="9">
-        <v>89</v>
+        <v>83.3</v>
       </c>
       <c r="E32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F32" s="9">
-        <f t="shared" si="1"/>
+        <f>SUM(D32,D40,D48)</f>
         <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C33">
         <v>2017</v>
       </c>
       <c r="D33" s="9">
-        <v>93.8</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="11">
-        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="F33" s="9">
+        <f>SUM(D33,D41,D49)</f>
         <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C34">
         <v>2017</v>
       </c>
-      <c r="D34" s="10">
-        <v>81.599999999999994</v>
+      <c r="D34" s="9">
+        <v>6.8</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" s="9">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C35">
         <v>2017</v>
       </c>
       <c r="D35" s="9">
-        <v>80.099999999999994</v>
+        <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
-      </c>
-      <c r="F35" s="9">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C36">
         <v>2017</v>
       </c>
       <c r="D36" s="9">
-        <v>83.3</v>
+        <v>0.5</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
-      </c>
-      <c r="F36" s="9">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C37">
         <v>2017</v>
       </c>
       <c r="D37" s="9">
-        <v>78.400000000000006</v>
+        <v>2.5</v>
       </c>
       <c r="E37" t="s">
-        <v>37</v>
-      </c>
-      <c r="F37" s="9">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C38">
         <v>2017</v>
       </c>
       <c r="D38" s="9">
-        <v>6.8</v>
+        <v>7.5</v>
       </c>
       <c r="E38" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C39">
         <v>2017</v>
       </c>
       <c r="D39" s="9">
-        <v>4</v>
+        <v>5.2</v>
       </c>
       <c r="E39" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C40">
         <v>2017</v>
       </c>
       <c r="D40" s="9">
-        <v>0.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E40" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C41">
         <v>2017</v>
       </c>
       <c r="D41" s="9">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C42">
         <v>2017</v>
       </c>
       <c r="D42" s="9">
-        <v>3.9</v>
+        <v>6.3</v>
       </c>
       <c r="E42" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C43">
         <v>2017</v>
       </c>
       <c r="D43" s="9">
-        <v>7.5</v>
+        <v>10.7</v>
       </c>
       <c r="E43" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C44">
         <v>2017</v>
       </c>
       <c r="D44" s="9">
-        <v>5.2</v>
+        <v>7.5</v>
       </c>
       <c r="E44" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C45">
         <v>2017</v>
       </c>
       <c r="D45" s="9">
-        <v>4.9000000000000004</v>
+        <v>8.5</v>
       </c>
       <c r="E45" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C46">
         <v>2017</v>
       </c>
       <c r="D46" s="9">
-        <v>6</v>
+        <v>10.9</v>
       </c>
       <c r="E46" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C47">
         <v>2017</v>
       </c>
       <c r="D47" s="9">
-        <v>6.3</v>
+        <v>14.7</v>
       </c>
       <c r="E47" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C48">
         <v>2017</v>
       </c>
       <c r="D48" s="9">
-        <v>10.7</v>
+        <v>11.8</v>
       </c>
       <c r="E48" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C49">
         <v>2017</v>
       </c>
       <c r="D49" s="9">
-        <v>7.5</v>
+        <v>15.6</v>
       </c>
       <c r="E49" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C50">
         <v>2017</v>
       </c>
       <c r="D50" s="9">
-        <v>8.5</v>
+        <v>55.3</v>
       </c>
       <c r="E50" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="F50" s="9">
+        <f>SUM(D50,D58,D66)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C51">
         <v>2017</v>
       </c>
       <c r="D51" s="9">
-        <v>2.2999999999999998</v>
+        <v>54.5</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="F51" s="9">
+        <f>SUM(D51,D59,D67)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C52">
         <v>2017</v>
       </c>
       <c r="D52" s="9">
-        <v>10.9</v>
+        <v>55.4</v>
       </c>
       <c r="E52" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="F52" s="9">
+        <f>SUM(D52,D60,D68)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C53">
         <v>2017</v>
       </c>
       <c r="D53" s="9">
-        <v>14.7</v>
+        <v>56.1</v>
       </c>
       <c r="E53" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="F53" s="9">
+        <f>SUM(D53,D61,D69)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C54">
         <v>2017</v>
       </c>
-      <c r="D54" s="9">
-        <v>11.8</v>
+      <c r="D54" s="10">
+        <v>24.8</v>
       </c>
       <c r="E54" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="F54" s="11">
+        <f>SUM(D54,D62,D70)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C55">
         <v>2017</v>
       </c>
       <c r="D55" s="9">
-        <v>15.6</v>
+        <v>47.1</v>
       </c>
       <c r="E55" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="F55" s="9">
+        <f>SUM(D55,D63,D71)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C56">
         <v>2017</v>
       </c>
       <c r="D56" s="9">
-        <v>55.3</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="E56" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F56" s="9">
-        <f>SUM(D56,D65,D74)</f>
+        <f>SUM(D56,D64,D72)</f>
         <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C57">
         <v>2017</v>
       </c>
       <c r="D57" s="9">
-        <v>54.5</v>
+        <v>45.8</v>
       </c>
       <c r="E57" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F57" s="9">
-        <f t="shared" ref="F57:F64" si="2">SUM(D57,D66,D75)</f>
+        <f>SUM(D57,D65,D73)</f>
         <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C58">
         <v>2017</v>
       </c>
       <c r="D58" s="9">
-        <v>55.4</v>
+        <v>24.1</v>
       </c>
       <c r="E58" t="s">
-        <v>40</v>
-      </c>
-      <c r="F58" s="9">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B59" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C59">
         <v>2017</v>
       </c>
       <c r="D59" s="9">
-        <v>56.1</v>
+        <v>6.9</v>
       </c>
       <c r="E59" t="s">
-        <v>41</v>
-      </c>
-      <c r="F59" s="9">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C60">
         <v>2017</v>
       </c>
       <c r="D60" s="9">
-        <v>62</v>
+        <v>6.8</v>
       </c>
       <c r="E60" t="s">
-        <v>42</v>
-      </c>
-      <c r="F60" s="9">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C61">
         <v>2017</v>
       </c>
-      <c r="D61" s="10">
-        <v>24.8</v>
+      <c r="D61" s="9">
+        <v>9.9</v>
       </c>
       <c r="E61" t="s">
-        <v>43</v>
-      </c>
-      <c r="F61" s="11">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C62">
         <v>2017</v>
       </c>
       <c r="D62" s="9">
-        <v>47.1</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E62" t="s">
-        <v>44</v>
-      </c>
-      <c r="F62" s="9">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B63" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C63">
         <v>2017</v>
       </c>
       <c r="D63" s="9">
-        <v>37.700000000000003</v>
+        <v>15.9</v>
       </c>
       <c r="E63" t="s">
-        <v>45</v>
-      </c>
-      <c r="F63" s="9">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C64">
         <v>2017</v>
       </c>
       <c r="D64" s="9">
-        <v>45.8</v>
+        <v>13.2</v>
       </c>
       <c r="E64" t="s">
-        <v>46</v>
-      </c>
-      <c r="F64" s="9">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65">
+        <v>2017</v>
+      </c>
+      <c r="D65" s="9">
+        <v>12.4</v>
+      </c>
+      <c r="E65" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" t="s">
         <v>11</v>
       </c>
-      <c r="C65">
-        <v>2017</v>
-      </c>
-      <c r="D65" s="9">
-        <v>24.1</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="C66">
+        <v>2017</v>
+      </c>
+      <c r="D66" s="9">
+        <v>20.6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67">
+        <v>2017</v>
+      </c>
+      <c r="D67" s="9">
+        <v>38.6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68">
+        <v>2017</v>
+      </c>
+      <c r="D68" s="9">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E68" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69">
+        <v>2017</v>
+      </c>
+      <c r="D69" s="9">
+        <v>34</v>
+      </c>
+      <c r="E69" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>83</v>
-      </c>
-      <c r="B66" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66">
-        <v>2017</v>
-      </c>
-      <c r="D66" s="9">
-        <v>6.9</v>
-      </c>
-      <c r="E66" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70">
+        <v>2017</v>
+      </c>
+      <c r="D70" s="9">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="E70" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>83</v>
-      </c>
-      <c r="B67" t="s">
-        <v>13</v>
-      </c>
-      <c r="C67">
-        <v>2017</v>
-      </c>
-      <c r="D67" s="9">
-        <v>6.8</v>
-      </c>
-      <c r="E67" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71">
+        <v>2017</v>
+      </c>
+      <c r="D71" s="9">
+        <v>37</v>
+      </c>
+      <c r="E71" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>83</v>
-      </c>
-      <c r="B68" t="s">
-        <v>14</v>
-      </c>
-      <c r="C68">
-        <v>2017</v>
-      </c>
-      <c r="D68" s="9">
-        <v>9.9</v>
-      </c>
-      <c r="E68" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72">
+        <v>2017</v>
+      </c>
+      <c r="D72" s="9">
+        <v>49.1</v>
+      </c>
+      <c r="E72" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>83</v>
-      </c>
-      <c r="B69" t="s">
-        <v>15</v>
-      </c>
-      <c r="C69">
-        <v>2017</v>
-      </c>
-      <c r="D69" s="9">
-        <v>10.1</v>
-      </c>
-      <c r="E69" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73">
+        <v>2017</v>
+      </c>
+      <c r="D73" s="9">
+        <v>41.8</v>
+      </c>
+      <c r="E73" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>83</v>
-      </c>
-      <c r="B70" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70">
-        <v>2017</v>
-      </c>
-      <c r="D70" s="9">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E70" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>83</v>
-      </c>
-      <c r="B71" t="s">
-        <v>17</v>
-      </c>
-      <c r="C71">
-        <v>2017</v>
-      </c>
-      <c r="D71" s="9">
-        <v>15.9</v>
-      </c>
-      <c r="E71" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" t="s">
-        <v>18</v>
-      </c>
-      <c r="C72">
-        <v>2017</v>
-      </c>
-      <c r="D72" s="9">
-        <v>13.2</v>
-      </c>
-      <c r="E72" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>83</v>
-      </c>
-      <c r="B73" t="s">
-        <v>19</v>
-      </c>
-      <c r="C73">
-        <v>2017</v>
-      </c>
-      <c r="D73" s="9">
-        <v>12.4</v>
-      </c>
-      <c r="E73" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B74" t="s">
         <v>11</v>
@@ -2071,15 +2038,19 @@
         <v>2017</v>
       </c>
       <c r="D74" s="9">
-        <v>20.6</v>
+        <v>84</v>
       </c>
       <c r="E74" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="F74" s="9">
+        <f>SUM(D74,D82,D90)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B75" t="s">
         <v>12</v>
@@ -2088,15 +2059,19 @@
         <v>2017</v>
       </c>
       <c r="D75" s="9">
-        <v>38.6</v>
+        <v>86</v>
       </c>
       <c r="E75" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="F75" s="9">
+        <f>SUM(D75,D83,D91)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
         <v>13</v>
@@ -2105,15 +2080,19 @@
         <v>2017</v>
       </c>
       <c r="D76" s="9">
-        <v>37.799999999999997</v>
+        <v>47</v>
       </c>
       <c r="E76" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="F76" s="9">
+        <f>SUM(D76,D84,D92)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B77" t="s">
         <v>14</v>
@@ -2122,15 +2101,19 @@
         <v>2017</v>
       </c>
       <c r="D77" s="9">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="E77" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="F77" s="9">
+        <f>SUM(D77,D85,D93)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B78" t="s">
         <v>15</v>
@@ -2139,15 +2122,19 @@
         <v>2017</v>
       </c>
       <c r="D78" s="9">
-        <v>27.9</v>
+        <v>82</v>
       </c>
       <c r="E78" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="F78" s="9">
+        <f>SUM(D78,D86,D94)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>16</v>
@@ -2156,15 +2143,19 @@
         <v>2017</v>
       </c>
       <c r="D79" s="9">
-        <v>66.400000000000006</v>
+        <v>67</v>
       </c>
       <c r="E79" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="F79" s="9">
+        <f>SUM(D79,D87,D95)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
         <v>17</v>
@@ -2173,15 +2164,19 @@
         <v>2017</v>
       </c>
       <c r="D80" s="9">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="E80" t="s">
         <v>44</v>
       </c>
+      <c r="F80" s="9">
+        <f>SUM(D80,D88,D96)</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
         <v>18</v>
@@ -2190,24 +2185,28 @@
         <v>2017</v>
       </c>
       <c r="D81" s="9">
-        <v>49.1</v>
+        <v>53</v>
       </c>
       <c r="E81" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="F81" s="9">
+        <f>SUM(D81,D89,D97)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C82">
         <v>2017</v>
       </c>
       <c r="D82" s="9">
-        <v>41.8</v>
+        <v>4</v>
       </c>
       <c r="E82" t="s">
         <v>46</v>
@@ -2215,205 +2214,169 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B83" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C83">
         <v>2017</v>
       </c>
       <c r="D83" s="9">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="E83" t="s">
-        <v>50</v>
-      </c>
-      <c r="F83" s="9">
-        <f>SUM(D83,D92,D101)</f>
-        <v>100</v>
+        <v>45</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B84" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C84">
         <v>2017</v>
       </c>
       <c r="D84" s="9">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="E84" t="s">
-        <v>49</v>
-      </c>
-      <c r="F84" s="9">
-        <f t="shared" ref="F84:F91" si="3">SUM(D84,D93,D102)</f>
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C85">
         <v>2017</v>
       </c>
       <c r="D85" s="9">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>55</v>
-      </c>
-      <c r="F85" s="9">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <v>48</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B86" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C86">
         <v>2017</v>
       </c>
       <c r="D86" s="9">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="E86" t="s">
-        <v>53</v>
-      </c>
-      <c r="F86" s="9">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B87" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C87">
         <v>2017</v>
       </c>
       <c r="D87" s="9">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="E87" t="s">
-        <v>52</v>
-      </c>
-      <c r="F87" s="9">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B88" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C88">
         <v>2017</v>
       </c>
       <c r="D88" s="9">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>54</v>
-      </c>
-      <c r="F88" s="9">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <v>44</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B89" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C89">
         <v>2017</v>
       </c>
       <c r="D89" s="9">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="E89" t="s">
-        <v>51</v>
-      </c>
-      <c r="F89" s="9">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <v>43</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B90" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C90">
         <v>2017</v>
       </c>
       <c r="D90" s="9">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="E90" t="s">
-        <v>48</v>
-      </c>
-      <c r="F90" s="9">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B91" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C91">
         <v>2017</v>
       </c>
       <c r="D91" s="9">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="E91" t="s">
-        <v>47</v>
-      </c>
-      <c r="F91" s="9">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <v>45</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B92" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C92">
         <v>2017</v>
       </c>
       <c r="D92" s="9">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="E92" t="s">
         <v>50</v>
@@ -2421,10 +2384,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B93" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C93">
         <v>2017</v>
@@ -2433,499 +2396,495 @@
         <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B94" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C94">
         <v>2017</v>
       </c>
       <c r="D94" s="9">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E94" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B95" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C95">
         <v>2017</v>
       </c>
       <c r="D95" s="9">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E95" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B96" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C96">
         <v>2017</v>
       </c>
       <c r="D96" s="9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E96" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B97" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C97">
         <v>2017</v>
       </c>
       <c r="D97" s="9">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="E97" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B98" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C98">
         <v>2017</v>
       </c>
       <c r="D98" s="9">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="E98" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="F98" s="11">
+        <f>SUM(D98,D106,D114)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B99" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C99">
         <v>2017</v>
       </c>
       <c r="D99" s="9">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E99" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+      <c r="F99" s="9">
+        <f>SUM(D99,D107,D115)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B100" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C100">
         <v>2017</v>
       </c>
       <c r="D100" s="9">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="E100" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="F100" s="9">
+        <f>SUM(D100,D108,D116)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B101" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C101">
         <v>2017</v>
       </c>
       <c r="D101" s="9">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="E101" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="F101" s="9">
+        <f>SUM(D101,D109,D117)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B102" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C102">
         <v>2017</v>
       </c>
       <c r="D102" s="9">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="E102" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="F102" s="9">
+        <f>SUM(D102,D110,D118)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B103" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C103">
         <v>2017</v>
       </c>
       <c r="D103" s="9">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="E103" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="F103" s="9">
+        <f>SUM(D103,D111,D119)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B104" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C104">
         <v>2017</v>
       </c>
       <c r="D104" s="9">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="E104" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+      <c r="F104" s="9">
+        <f>SUM(D104,D112,D120)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B105" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C105">
         <v>2017</v>
       </c>
       <c r="D105" s="9">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="E105" t="s">
-        <v>52</v>
+        <v>57</v>
+      </c>
+      <c r="F105" s="11">
+        <f>SUM(D105,D113,D121)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B106" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C106">
         <v>2017</v>
       </c>
       <c r="D106" s="9">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E106" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B107" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C107">
         <v>2017</v>
       </c>
       <c r="D107" s="9">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E107" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B108" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C108">
         <v>2017</v>
       </c>
       <c r="D108" s="9">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E108" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B109" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C109">
         <v>2017</v>
       </c>
       <c r="D109" s="9">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E109" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B110" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C110">
         <v>2017</v>
       </c>
       <c r="D110" s="9">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="E110" t="s">
-        <v>57</v>
-      </c>
-      <c r="F110" s="11">
-        <f>SUM(D110,D119,D128)</f>
-        <v>100</v>
+        <v>51</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B111" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C111">
         <v>2017</v>
       </c>
       <c r="D111" s="9">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="E111" t="s">
-        <v>58</v>
-      </c>
-      <c r="F111" s="9">
-        <f t="shared" ref="F111:F118" si="4">SUM(D111,D120,D129)</f>
-        <v>100</v>
+        <v>56</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B112" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C112">
         <v>2017</v>
       </c>
       <c r="D112" s="9">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E112" t="s">
-        <v>59</v>
-      </c>
-      <c r="F112" s="9">
-        <f t="shared" si="4"/>
-        <v>100</v>
+        <v>58</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B113" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C113">
         <v>2017</v>
       </c>
-      <c r="D113" s="9">
-        <v>95</v>
+      <c r="D113" s="10">
+        <v>6</v>
       </c>
       <c r="E113" t="s">
-        <v>60</v>
-      </c>
-      <c r="F113" s="9">
-        <f t="shared" si="4"/>
-        <v>100</v>
+        <v>57</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B114" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C114">
         <v>2017</v>
       </c>
-      <c r="D114" s="9">
-        <v>67</v>
+      <c r="D114" s="10">
+        <v>13</v>
       </c>
       <c r="E114" t="s">
-        <v>61</v>
-      </c>
-      <c r="F114" s="9">
-        <f t="shared" si="4"/>
-        <v>100</v>
+        <v>52</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B115" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C115">
         <v>2017</v>
       </c>
       <c r="D115" s="9">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="E115" t="s">
-        <v>56</v>
-      </c>
-      <c r="F115" s="9">
-        <f t="shared" si="4"/>
-        <v>100</v>
+        <v>53</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B116" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C116">
         <v>2017</v>
       </c>
       <c r="D116" s="9">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="E116" t="s">
-        <v>62</v>
-      </c>
-      <c r="F116" s="9">
-        <f t="shared" si="4"/>
-        <v>100</v>
+        <v>54</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B117" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C117">
         <v>2017</v>
       </c>
       <c r="D117" s="9">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="E117" t="s">
-        <v>64</v>
-      </c>
-      <c r="F117" s="9">
-        <f t="shared" si="4"/>
-        <v>100</v>
+        <v>55</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C118">
         <v>2017</v>
       </c>
       <c r="D118" s="9">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="E118" t="s">
-        <v>63</v>
-      </c>
-      <c r="F118" s="11">
-        <f t="shared" si="4"/>
-        <v>100</v>
+        <v>51</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B119" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C119">
         <v>2017</v>
       </c>
       <c r="D119" s="9">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="E119" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B120" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C120">
         <v>2017</v>
       </c>
       <c r="D120" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E120" t="s">
         <v>58</v>
@@ -2933,769 +2892,459 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B121" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C121">
         <v>2017</v>
       </c>
       <c r="D121" s="9">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="E121" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B122" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C122">
         <v>2017</v>
       </c>
       <c r="D122" s="9">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="E122" t="s">
         <v>60</v>
       </c>
+      <c r="F122" s="9">
+        <f>SUM(D122,D130,D138)</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B123" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C123">
         <v>2017</v>
       </c>
       <c r="D123" s="9">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="E123" t="s">
         <v>61</v>
       </c>
+      <c r="F123" s="9">
+        <f>SUM(D123,D131,D139)</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B124" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C124">
         <v>2017</v>
       </c>
       <c r="D124" s="9">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="E124" t="s">
-        <v>56</v>
+        <v>62</v>
+      </c>
+      <c r="F124" s="9">
+        <f>SUM(D124,D132,D140)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B125" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C125">
         <v>2017</v>
       </c>
       <c r="D125" s="9">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="E125" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="F125" s="9">
+        <f>SUM(D125,D133,D141)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B126" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C126">
         <v>2017</v>
       </c>
       <c r="D126" s="9">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="E126" t="s">
         <v>64</v>
       </c>
+      <c r="F126" s="9">
+        <f>SUM(D126,D134,D142)</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B127" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C127">
         <v>2017</v>
       </c>
-      <c r="D127" s="10">
-        <v>6</v>
+      <c r="D127" s="9">
+        <v>92</v>
       </c>
       <c r="E127" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="F127" s="9">
+        <f>SUM(D127,D135,D143)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B128" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C128">
         <v>2017</v>
       </c>
-      <c r="D128" s="10">
-        <v>13</v>
+      <c r="D128" s="9">
+        <v>95</v>
       </c>
       <c r="E128" t="s">
-        <v>57</v>
+        <v>66</v>
+      </c>
+      <c r="F128" s="9">
+        <f>SUM(D128,D136,D144)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B129" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C129">
         <v>2017</v>
       </c>
       <c r="D129" s="9">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="E129" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="F129" s="9">
+        <f>SUM(D129,D137,D145)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B130" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C130">
         <v>2017</v>
       </c>
       <c r="D130" s="9">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="E130" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B131" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C131">
         <v>2017</v>
       </c>
       <c r="D131" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E131" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B132" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C132">
         <v>2017</v>
       </c>
       <c r="D132" s="9">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E132" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B133" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C133">
         <v>2017</v>
       </c>
       <c r="D133" s="9">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E133" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B134" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C134">
         <v>2017</v>
       </c>
       <c r="D134" s="9">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E134" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B135" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C135">
         <v>2017</v>
       </c>
       <c r="D135" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E135" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B136" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C136">
         <v>2017</v>
       </c>
       <c r="D136" s="9">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="E136" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B137" t="s">
+        <v>18</v>
+      </c>
+      <c r="C137">
+        <v>2017</v>
+      </c>
+      <c r="D137" s="9">
         <v>11</v>
       </c>
-      <c r="C137">
-        <v>2017</v>
-      </c>
-      <c r="D137" s="9">
-        <v>85</v>
-      </c>
       <c r="E137" t="s">
-        <v>66</v>
-      </c>
-      <c r="F137" s="9">
-        <f>SUM(D137,D146,D155)</f>
-        <v>100</v>
+        <v>59</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B138" t="s">
+        <v>11</v>
+      </c>
+      <c r="C138">
+        <v>2017</v>
+      </c>
+      <c r="D138" s="9">
         <v>12</v>
       </c>
-      <c r="C138">
-        <v>2017</v>
-      </c>
-      <c r="D138" s="9">
-        <v>91</v>
-      </c>
       <c r="E138" t="s">
-        <v>67</v>
-      </c>
-      <c r="F138" s="9">
-        <f t="shared" ref="F138:F145" si="5">SUM(D138,D147,D156)</f>
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B139" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C139">
         <v>2017</v>
       </c>
       <c r="D139" s="9">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="E139" t="s">
-        <v>68</v>
-      </c>
-      <c r="F139" s="9">
-        <f t="shared" si="5"/>
-        <v>100</v>
+        <v>61</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B140" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C140">
         <v>2017</v>
       </c>
       <c r="D140" s="9">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="E140" t="s">
-        <v>69</v>
-      </c>
-      <c r="F140" s="9">
-        <f t="shared" si="5"/>
-        <v>100</v>
+        <v>62</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B141" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C141">
         <v>2017</v>
       </c>
       <c r="D141" s="9">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="E141" t="s">
-        <v>70</v>
-      </c>
-      <c r="F141" s="9">
-        <f t="shared" si="5"/>
-        <v>100</v>
+        <v>63</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B142" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C142">
         <v>2017</v>
       </c>
       <c r="D142" s="9">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="E142" t="s">
-        <v>71</v>
-      </c>
-      <c r="F142" s="9">
-        <f t="shared" si="5"/>
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B143" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C143">
         <v>2017</v>
       </c>
       <c r="D143" s="9">
-        <v>92</v>
+        <v>3</v>
       </c>
       <c r="E143" t="s">
-        <v>72</v>
-      </c>
-      <c r="F143" s="9">
-        <f t="shared" si="5"/>
-        <v>100</v>
+        <v>65</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B144" t="s">
+        <v>17</v>
+      </c>
+      <c r="C144">
+        <v>2017</v>
+      </c>
+      <c r="D144" s="9">
+        <v>3</v>
+      </c>
+      <c r="E144" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>86</v>
+      </c>
+      <c r="B145" t="s">
         <v>18</v>
       </c>
-      <c r="C144">
-        <v>2017</v>
-      </c>
-      <c r="D144" s="9">
-        <v>95</v>
-      </c>
-      <c r="E144" t="s">
-        <v>73</v>
-      </c>
-      <c r="F144" s="9">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>91</v>
-      </c>
-      <c r="B145" t="s">
-        <v>19</v>
-      </c>
       <c r="C145">
         <v>2017</v>
       </c>
       <c r="D145" s="9">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="E145" t="s">
-        <v>65</v>
-      </c>
-      <c r="F145" s="9">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>92</v>
-      </c>
-      <c r="B146" t="s">
-        <v>11</v>
-      </c>
-      <c r="C146">
-        <v>2017</v>
-      </c>
-      <c r="D146" s="9">
-        <v>3</v>
-      </c>
-      <c r="E146" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>92</v>
-      </c>
-      <c r="B147" t="s">
-        <v>12</v>
-      </c>
-      <c r="C147">
-        <v>2017</v>
-      </c>
-      <c r="D147" s="9">
-        <v>1</v>
-      </c>
-      <c r="E147" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
-        <v>92</v>
-      </c>
-      <c r="B148" t="s">
-        <v>13</v>
-      </c>
-      <c r="C148">
-        <v>2017</v>
-      </c>
-      <c r="D148" s="9">
-        <v>21</v>
-      </c>
-      <c r="E148" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>92</v>
-      </c>
-      <c r="B149" t="s">
-        <v>14</v>
-      </c>
-      <c r="C149">
-        <v>2017</v>
-      </c>
-      <c r="D149" s="9">
-        <v>1</v>
-      </c>
-      <c r="E149" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>92</v>
-      </c>
-      <c r="B150" t="s">
-        <v>15</v>
-      </c>
-      <c r="C150">
-        <v>2017</v>
-      </c>
-      <c r="D150" s="9">
-        <v>6</v>
-      </c>
-      <c r="E150" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
-        <v>92</v>
-      </c>
-      <c r="B151" t="s">
-        <v>16</v>
-      </c>
-      <c r="C151">
-        <v>2017</v>
-      </c>
-      <c r="D151" s="9">
-        <v>2</v>
-      </c>
-      <c r="E151" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
-        <v>92</v>
-      </c>
-      <c r="B152" t="s">
-        <v>17</v>
-      </c>
-      <c r="C152">
-        <v>2017</v>
-      </c>
-      <c r="D152" s="9">
-        <v>5</v>
-      </c>
-      <c r="E152" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
-        <v>92</v>
-      </c>
-      <c r="B153" t="s">
-        <v>18</v>
-      </c>
-      <c r="C153">
-        <v>2017</v>
-      </c>
-      <c r="D153" s="9">
-        <v>2</v>
-      </c>
-      <c r="E153" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
-        <v>92</v>
-      </c>
-      <c r="B154" t="s">
-        <v>19</v>
-      </c>
-      <c r="C154">
-        <v>2017</v>
-      </c>
-      <c r="D154" s="9">
-        <v>11</v>
-      </c>
-      <c r="E154" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>93</v>
-      </c>
-      <c r="B155" t="s">
-        <v>11</v>
-      </c>
-      <c r="C155">
-        <v>2017</v>
-      </c>
-      <c r="D155" s="9">
-        <v>12</v>
-      </c>
-      <c r="E155" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
-        <v>93</v>
-      </c>
-      <c r="B156" t="s">
-        <v>12</v>
-      </c>
-      <c r="C156">
-        <v>2017</v>
-      </c>
-      <c r="D156" s="9">
-        <v>8</v>
-      </c>
-      <c r="E156" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
-        <v>93</v>
-      </c>
-      <c r="B157" t="s">
-        <v>13</v>
-      </c>
-      <c r="C157">
-        <v>2017</v>
-      </c>
-      <c r="D157" s="9">
-        <v>17</v>
-      </c>
-      <c r="E157" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
-        <v>93</v>
-      </c>
-      <c r="B158" t="s">
-        <v>14</v>
-      </c>
-      <c r="C158">
-        <v>2017</v>
-      </c>
-      <c r="D158" s="9">
-        <v>1</v>
-      </c>
-      <c r="E158" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
-        <v>93</v>
-      </c>
-      <c r="B159" t="s">
-        <v>15</v>
-      </c>
-      <c r="C159">
-        <v>2017</v>
-      </c>
-      <c r="D159" s="9">
-        <v>26</v>
-      </c>
-      <c r="E159" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
-        <v>93</v>
-      </c>
-      <c r="B160" t="s">
-        <v>16</v>
-      </c>
-      <c r="C160">
-        <v>2017</v>
-      </c>
-      <c r="D160" s="9">
-        <v>11</v>
-      </c>
-      <c r="E160" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>93</v>
-      </c>
-      <c r="B161" t="s">
-        <v>17</v>
-      </c>
-      <c r="C161">
-        <v>2017</v>
-      </c>
-      <c r="D161" s="9">
-        <v>3</v>
-      </c>
-      <c r="E161" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>93</v>
-      </c>
-      <c r="B162" t="s">
-        <v>18</v>
-      </c>
-      <c r="C162">
-        <v>2017</v>
-      </c>
-      <c r="D162" s="9">
-        <v>3</v>
-      </c>
-      <c r="E162" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
-        <v>93</v>
-      </c>
-      <c r="B163" t="s">
-        <v>19</v>
-      </c>
-      <c r="C163">
-        <v>2017</v>
-      </c>
-      <c r="D163" s="9">
-        <v>35</v>
-      </c>
-      <c r="E163" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3732,7 +3381,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3740,7 +3389,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>